<commit_message>
made changes on t value
</commit_message>
<xml_diff>
--- a/papers/correlational analysis/age_social_distance.xlsx
+++ b/papers/correlational analysis/age_social_distance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Child ID</t>
   </si>
@@ -91,12 +91,33 @@
   <si>
     <t>age</t>
   </si>
+  <si>
+    <t>t-value</t>
+  </si>
+  <si>
+    <t>STAD DEV</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>Z_SCORE</t>
+  </si>
+  <si>
+    <t>MARGIN OF ERROR</t>
+  </si>
+  <si>
+    <t>SAMPLE SIZE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="181" formatCode="0.000000000000000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +137,14 @@
       <b/>
       <i/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -174,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -186,6 +215,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1610,11 +1644,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1347884768"/>
-        <c:axId val="-1347875520"/>
+        <c:axId val="-1083657184"/>
+        <c:axId val="-1083653376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1347884768"/>
+        <c:axId val="-1083657184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,12 +1704,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1347875520"/>
+        <c:crossAx val="-1083653376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1347875520"/>
+        <c:axId val="-1083653376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1765,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1347884768"/>
+        <c:crossAx val="-1083657184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3243,11 +3277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1342449616"/>
-        <c:axId val="-1342442000"/>
+        <c:axId val="-1083656640"/>
+        <c:axId val="-1083652288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1342449616"/>
+        <c:axId val="-1083656640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3304,12 +3338,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1342442000"/>
+        <c:crossAx val="-1083652288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1342442000"/>
+        <c:axId val="-1083652288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3360,7 +3394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1342449616"/>
+        <c:crossAx val="-1083656640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4570,16 +4604,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>504824</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>128589</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4901,7 +4935,7 @@
   <dimension ref="A1:Q215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16304,8 +16338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16355,7 +16389,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16401,20 +16435,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:F215"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="19.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.25" customWidth="1"/>
+    <col min="6" max="6" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16424,8 +16460,9 @@
       <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -16435,8 +16472,14 @@
       <c r="C2" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="8">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -16446,8 +16489,15 @@
       <c r="C3" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="6">
+        <f>TTEST($B$2:$B$215,$C$2:$C$215,1,2)</f>
+        <v>1.8506365106794279E-54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -16457,8 +16507,15 @@
       <c r="C4" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <f>_xlfn.STDEV.P($B$2:$B$215,$C$2:$C$215)</f>
+        <v>5.4787019456891635</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -16468,8 +16525,15 @@
       <c r="C5" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <f>AVERAGE(B2:B215)</f>
+        <v>12.878504672897197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -16479,8 +16543,15 @@
       <c r="C6" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <f>STANDARDIZE(B2,F5,F4)</f>
+        <v>-0.3428740405152485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -16490,8 +16561,15 @@
       <c r="C7" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7">
+        <f>F6*(F4/SQRT(F2))</f>
+        <v>-0.1281129553584722</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -16502,7 +16580,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -16513,7 +16591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -16524,7 +16602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -16535,7 +16613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -16546,7 +16624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -16557,7 +16635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -16568,7 +16646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -16579,7 +16657,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>17</v>
       </c>
@@ -18781,6 +18859,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>